<commit_message>
Auth mit FB SignIn/ Sign Out
</commit_message>
<xml_diff>
--- a/doc/2022-03-11 Table in PlutoWeb.xlsx
+++ b/doc/2022-03-11 Table in PlutoWeb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawlandshutde-my.sharepoint.com/personal/dgreipl_az_haw-landshut_de/Documents/00 Module/.VL63 Mobile Technologies/PlutoWeb/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8195B11-2012-4353-9174-2E342F92D9E2}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BA840D-1553-45E3-BAC2-158E5DCF2E0B}"/>
   <bookViews>
-    <workbookView xWindow="24228" yWindow="2004" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23772" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Areas</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>si_button_sign_in</t>
+  </si>
+  <si>
+    <t>ac_button_delete_account</t>
+  </si>
+  <si>
+    <t>areaAccount</t>
+  </si>
+  <si>
+    <t>ac_email</t>
+  </si>
+  <si>
+    <t>ac_verified</t>
   </si>
 </sst>
 </file>
@@ -410,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C21"/>
+  <dimension ref="B3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,10 +523,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B21" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Firestore write ok, reading still missing
</commit_message>
<xml_diff>
--- a/doc/2022-03-11 Table in PlutoWeb.xlsx
+++ b/doc/2022-03-11 Table in PlutoWeb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawlandshutde-my.sharepoint.com/personal/dgreipl_az_haw-landshut_de/Documents/00 Module/.VL63 Mobile Technologies/PlutoWeb/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BA840D-1553-45E3-BAC2-158E5DCF2E0B}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98C685A5-3939-4C62-A234-AAF4E719B3BA}"/>
   <bookViews>
-    <workbookView xWindow="23772" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Areas</t>
   </si>
@@ -98,6 +98,33 @@
   </si>
   <si>
     <t>ac_verified</t>
+  </si>
+  <si>
+    <t>Navigation Items</t>
+  </si>
+  <si>
+    <t>nav_sign_out</t>
+  </si>
+  <si>
+    <t>nav_sign_in</t>
+  </si>
+  <si>
+    <t>nav_account</t>
+  </si>
+  <si>
+    <t>nav_pluto23</t>
+  </si>
+  <si>
+    <t>nav_home</t>
+  </si>
+  <si>
+    <t>me_div_messages</t>
+  </si>
+  <si>
+    <t>me_body_text</t>
+  </si>
+  <si>
+    <t>me_button_send</t>
   </si>
 </sst>
 </file>
@@ -422,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C23"/>
+  <dimension ref="B3:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +570,55 @@
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
beta 24.12.2022 lätuft mit Android vom 24.12.2022
</commit_message>
<xml_diff>
--- a/doc/2022-03-11 Table in PlutoWeb.xlsx
+++ b/doc/2022-03-11 Table in PlutoWeb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawlandshutde-my.sharepoint.com/personal/dgreipl_az_haw-landshut_de/Documents/00 Module/.VL63 Mobile Technologies/PlutoWeb/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98C685A5-3939-4C62-A234-AAF4E719B3BA}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_AD4DB114E441178AC67DF41AAED0E5EE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85162074-0757-4217-8BAE-8C5FE1468043}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="20556" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Areas</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>me_button_send</t>
+  </si>
+  <si>
+    <t>ac_button_verify_account</t>
+  </si>
+  <si>
+    <t>ac_verification_hint</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C31"/>
+  <dimension ref="B3:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,100 +529,119 @@
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C16" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C28" s="1" t="s">
+    <row r="33" spans="3:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C29" s="1" t="s">
+    <row r="34" spans="3:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C30" s="1" t="s">
+    <row r="35" spans="3:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C31" s="1" t="s">
+    <row r="36" spans="3:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C36" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>